<commit_message>
Wrote test_q.ipynb where efficiency of join_annotations is improved
</commit_message>
<xml_diff>
--- a/excel_with_scores.xlsx
+++ b/excel_with_scores.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="72">
   <si>
     <t>label</t>
   </si>
@@ -58,6 +58,21 @@
     <t>score</t>
   </si>
   <si>
+    <t>.B152: Stemming[1]|STM 1_2503_16_16</t>
+  </si>
+  <si>
+    <t>stm\_reaction_2503_18_26</t>
+  </si>
+  <si>
+    <t>.B152: Stemming_2503_29_33</t>
+  </si>
+  <si>
+    <t>.B152: Stemming[4]|STM 0_2503_29_33</t>
+  </si>
+  <si>
+    <t>.B152: Stemming[4]|STM 0_2503_32_33</t>
+  </si>
+  <si>
     <t>type\_Background_2546_0_12</t>
   </si>
   <si>
@@ -88,19 +103,13 @@
     <t>FAC 1_2570_46_47</t>
   </si>
   <si>
-    <t>.B152: Stemming[1]|STM 1_2503_16_16</t>
-  </si>
-  <si>
-    <t>stm\_reaction_2503_18_26</t>
-  </si>
-  <si>
-    <t>.B152: Stemming_2503_29_33</t>
-  </si>
-  <si>
-    <t>.B152: Stemming[4]|STM 0_2503_29_33</t>
-  </si>
-  <si>
-    <t>.B152: Stemming[4]|STM 0_2503_32_33</t>
+    <t>.B152: Stemming_2503_29_34</t>
+  </si>
+  <si>
+    <t>.B152: Stemming[3]|STM 0_2503_29_34</t>
+  </si>
+  <si>
+    <t>.B152: Stemming[3]|STM 0_2503_32_32</t>
   </si>
   <si>
     <t>.D450: Lopen en zich verplaat_2570_45_45</t>
@@ -109,7 +118,28 @@
     <t>FAC 2_2570_46_50</t>
   </si>
   <si>
-    <t>_2503_0_35</t>
+    <t>type\_Background[2]|type\_Background_2546_14_35</t>
+  </si>
+  <si>
+    <t>type\_Background[2]|type\_Background[3]|.D450: Lopen en zich verplaatsen_2546_14_35</t>
+  </si>
+  <si>
+    <t>type\_Background[2]|type\_Background[3]|FAC 3[5]|type\_Implicit_2546_14_35</t>
+  </si>
+  <si>
+    <t>FAC 4_2570_46_50</t>
+  </si>
+  <si>
+    <t>.B152: Stemming[1]|STM 1</t>
+  </si>
+  <si>
+    <t>stm\_reaction</t>
+  </si>
+  <si>
+    <t>.B152: Stemming</t>
+  </si>
+  <si>
+    <t>.B152: Stemming[4]|STM 0</t>
   </si>
   <si>
     <t>type\_Background</t>
@@ -127,37 +157,49 @@
     <t>FAC 1</t>
   </si>
   <si>
-    <t>.B152: Stemming[1]|STM 1</t>
-  </si>
-  <si>
-    <t>stm\_reaction</t>
-  </si>
-  <si>
-    <t>.B152: Stemming</t>
-  </si>
-  <si>
-    <t>.B152: Stemming[4]|STM 0</t>
+    <t>.B152: Stemming[3]|STM 0</t>
   </si>
   <si>
     <t>FAC 2</t>
   </si>
   <si>
+    <t>type\_Background[2]|type\_Background</t>
+  </si>
+  <si>
+    <t>type\_Background[2]|type\_Background[3]|.D450: Lopen en zich verplaatsen</t>
+  </si>
+  <si>
+    <t>type\_Background[2]|type\_Background[3]|FAC 3[5]|type\_Implicit</t>
+  </si>
+  <si>
+    <t>FAC 4</t>
+  </si>
+  <si>
+    <t>2503</t>
+  </si>
+  <si>
     <t>2546</t>
   </si>
   <si>
     <t>2570</t>
   </si>
   <si>
-    <t>2503</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Op Dd-mm-jjjj zag ik bovengenoemde patiënt op de polikliniek radiotherapie van het ziekenhuis</t>
+    <t xml:space="preserve"> emotioneel</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> schoonzoon hoort morgen de uitslag van een aantal onderzoeken</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> maakt zich hier veel zorgen</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Op Dd-mm-jjjj zag ik bovengenoemde patiÃ«nt op de polikliniek radiotherapie van het ziekenhuis</t>
   </si>
   <si>
     <t xml:space="preserve"> 80 mg prednison als gevolg van ipi/nivo DM door prednisolon jjjj/mm : lopen moeizamer , blinde vlek en meerdere malen gevallen .</t>
   </si>
   <si>
-    <t xml:space="preserve"> Op Dd-mm-jjjj werd bovengenoemde patiënt gezien op de polikliniek revalidatiegeneeskunde op verzoek van voornaam achternaam , revalidatiearts voor advies bij spasticiteitsbehandeling en verbeteren looppatroon .</t>
+    <t xml:space="preserve"> Op Dd-mm-jjjj werd bovengenoemde patiÃ«nt gezien op de polikliniek revalidatiegeneeskunde op verzoek van voornaam achternaam , revalidatiearts voor advies bij spasticiteitsbehandeling en verbeteren looppatroon .</t>
   </si>
   <si>
     <t xml:space="preserve"> Na Ski ongeval met dwarslaesie tot gevolg in maanden jjjj heeft mevrouw 7 maanden intern moeten revalideren in locatie .</t>
@@ -169,13 +211,7 @@
     <t xml:space="preserve"> met rollator</t>
   </si>
   <si>
-    <t xml:space="preserve"> emotioneel</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> schoonzoon hoort morgen de uitslag van een aantal onderzoeken</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> maakt zich hier veel zorgen</t>
+    <t xml:space="preserve"> maakt zich hier veel zorgen om</t>
   </si>
   <si>
     <t xml:space="preserve"> lopen</t>
@@ -184,7 +220,7 @@
     <t xml:space="preserve"> met rollator binnen en buitenshuis</t>
   </si>
   <si>
-    <t xml:space="preserve"> NF : Pijn in de rug , verlicht met warme handdoek en pcm . Mw was emotioneel , schoonzoon hoort morgen de uitslag van een aantal onderzoeken en mw maakt zich hier veel zorgen om .</t>
+    <t xml:space="preserve"> veel zorgen</t>
   </si>
   <si>
     <t xml:space="preserve"> lopen moeizamer</t>
@@ -193,7 +229,7 @@
     <t xml:space="preserve"> dwarslaesie</t>
   </si>
   <si>
-    <t xml:space="preserve"> veel zorgen</t>
+    <t xml:space="preserve"> veel</t>
   </si>
 </sst>
 </file>
@@ -551,7 +587,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O19"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -606,31 +642,46 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E2">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>45</v>
+        <v>56</v>
+      </c>
+      <c r="G2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2">
+        <v>16</v>
+      </c>
+      <c r="J2">
+        <v>16</v>
+      </c>
+      <c r="K2" t="s">
+        <v>56</v>
       </c>
       <c r="L2">
         <v>1</v>
       </c>
       <c r="M2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N2">
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -638,31 +689,31 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="D3">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E3">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="L3">
         <v>1</v>
       </c>
       <c r="M3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N3">
         <v>0</v>
       </c>
       <c r="O3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -670,34 +721,19 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4">
+        <v>29</v>
+      </c>
+      <c r="E4">
         <v>33</v>
       </c>
-      <c r="C4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4">
-        <v>14</v>
-      </c>
-      <c r="E4">
-        <v>35</v>
-      </c>
       <c r="F4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I4">
-        <v>26</v>
-      </c>
-      <c r="J4">
-        <v>27</v>
-      </c>
-      <c r="K4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="L4">
         <v>1</v>
@@ -717,34 +753,34 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5">
+        <v>29</v>
+      </c>
+      <c r="E5">
         <v>33</v>
       </c>
-      <c r="C5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5">
-        <v>14</v>
-      </c>
-      <c r="E5">
-        <v>35</v>
-      </c>
       <c r="F5" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="G5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" t="s">
+        <v>53</v>
+      </c>
+      <c r="I5">
+        <v>32</v>
+      </c>
+      <c r="J5">
         <v>33</v>
       </c>
-      <c r="H5" t="s">
-        <v>42</v>
-      </c>
-      <c r="I5">
-        <v>26</v>
-      </c>
-      <c r="J5">
-        <v>27</v>
-      </c>
       <c r="K5" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="L5">
         <v>1</v>
@@ -764,19 +800,34 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6">
+        <v>29</v>
+      </c>
+      <c r="E6">
+        <v>33</v>
+      </c>
+      <c r="F6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" t="s">
+        <v>53</v>
+      </c>
+      <c r="I6">
         <v>32</v>
       </c>
-      <c r="C6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>24</v>
-      </c>
-      <c r="F6" t="s">
-        <v>47</v>
+      <c r="J6">
+        <v>33</v>
+      </c>
+      <c r="K6" t="s">
+        <v>68</v>
       </c>
       <c r="L6">
         <v>1</v>
@@ -796,31 +847,31 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="D7">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="L7">
         <v>1</v>
       </c>
       <c r="M7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N7">
         <v>0</v>
       </c>
       <c r="O7">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -828,46 +879,31 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="D8">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="E8">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="F8" t="s">
-        <v>48</v>
-      </c>
-      <c r="G8" t="s">
-        <v>34</v>
-      </c>
-      <c r="H8" t="s">
-        <v>43</v>
-      </c>
-      <c r="I8">
-        <v>29</v>
-      </c>
-      <c r="J8">
-        <v>29</v>
-      </c>
-      <c r="K8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L8">
         <v>1</v>
       </c>
       <c r="M8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N8">
         <v>0</v>
       </c>
       <c r="O8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -875,34 +911,34 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9">
+        <v>14</v>
+      </c>
+      <c r="E9">
+        <v>35</v>
+      </c>
+      <c r="F9" t="s">
+        <v>60</v>
+      </c>
+      <c r="G9" t="s">
         <v>43</v>
       </c>
-      <c r="D9">
-        <v>25</v>
-      </c>
-      <c r="E9">
-        <v>44</v>
-      </c>
-      <c r="F9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G9" t="s">
-        <v>34</v>
-      </c>
       <c r="H9" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="I9">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J9">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K9" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="L9">
         <v>1</v>
@@ -922,19 +958,34 @@
         <v>22</v>
       </c>
       <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10">
+        <v>14</v>
+      </c>
+      <c r="E10">
         <v>35</v>
       </c>
-      <c r="C10" t="s">
+      <c r="F10" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" t="s">
         <v>43</v>
       </c>
-      <c r="D10">
-        <v>29</v>
-      </c>
-      <c r="E10">
-        <v>45</v>
-      </c>
-      <c r="F10" t="s">
-        <v>49</v>
+      <c r="H10" t="s">
+        <v>54</v>
+      </c>
+      <c r="I10">
+        <v>26</v>
+      </c>
+      <c r="J10">
+        <v>27</v>
+      </c>
+      <c r="K10" t="s">
+        <v>69</v>
       </c>
       <c r="L10">
         <v>1</v>
@@ -954,19 +1005,19 @@
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="D11">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="F11" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="L11">
         <v>1</v>
@@ -986,46 +1037,31 @@
         <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12">
+        <v>25</v>
+      </c>
+      <c r="E12">
         <v>44</v>
       </c>
-      <c r="D12">
-        <v>16</v>
-      </c>
-      <c r="E12">
-        <v>16</v>
-      </c>
       <c r="F12" t="s">
-        <v>51</v>
-      </c>
-      <c r="G12" t="s">
-        <v>37</v>
-      </c>
-      <c r="H12" t="s">
-        <v>44</v>
-      </c>
-      <c r="I12">
-        <v>16</v>
-      </c>
-      <c r="J12">
-        <v>16</v>
-      </c>
-      <c r="K12" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="L12">
         <v>1</v>
       </c>
       <c r="M12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O12">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -1033,19 +1069,34 @@
         <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13">
+        <v>25</v>
+      </c>
+      <c r="E13">
         <v>44</v>
       </c>
-      <c r="D13">
-        <v>18</v>
-      </c>
-      <c r="E13">
-        <v>26</v>
-      </c>
       <c r="F13" t="s">
-        <v>52</v>
+        <v>62</v>
+      </c>
+      <c r="G13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H13" t="s">
+        <v>55</v>
+      </c>
+      <c r="I13">
+        <v>29</v>
+      </c>
+      <c r="J13">
+        <v>29</v>
+      </c>
+      <c r="K13" t="s">
+        <v>70</v>
       </c>
       <c r="L13">
         <v>1</v>
@@ -1065,19 +1116,34 @@
         <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14">
+        <v>25</v>
+      </c>
+      <c r="E14">
         <v>44</v>
       </c>
-      <c r="D14">
+      <c r="F14" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" t="s">
+        <v>44</v>
+      </c>
+      <c r="H14" t="s">
+        <v>55</v>
+      </c>
+      <c r="I14">
         <v>29</v>
       </c>
-      <c r="E14">
-        <v>33</v>
-      </c>
-      <c r="F14" t="s">
-        <v>53</v>
+      <c r="J14">
+        <v>29</v>
+      </c>
+      <c r="K14" t="s">
+        <v>70</v>
       </c>
       <c r="L14">
         <v>1</v>
@@ -1097,34 +1163,19 @@
         <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="D15">
         <v>29</v>
       </c>
       <c r="E15">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="F15" t="s">
-        <v>53</v>
-      </c>
-      <c r="G15" t="s">
-        <v>40</v>
-      </c>
-      <c r="H15" t="s">
-        <v>44</v>
-      </c>
-      <c r="I15">
-        <v>32</v>
-      </c>
-      <c r="J15">
-        <v>33</v>
-      </c>
-      <c r="K15" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="L15">
         <v>1</v>
@@ -1144,34 +1195,19 @@
         <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="D16">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="E16">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="F16" t="s">
-        <v>53</v>
-      </c>
-      <c r="G16" t="s">
-        <v>40</v>
-      </c>
-      <c r="H16" t="s">
-        <v>44</v>
-      </c>
-      <c r="I16">
-        <v>32</v>
-      </c>
-      <c r="J16">
-        <v>33</v>
-      </c>
-      <c r="K16" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="L16">
         <v>1</v>
@@ -1191,19 +1227,19 @@
         <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="D17">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="E17">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="F17" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="L17">
         <v>0</v>
@@ -1223,19 +1259,34 @@
         <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="D18">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="E18">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="F18" t="s">
-        <v>55</v>
+        <v>65</v>
+      </c>
+      <c r="G18" t="s">
+        <v>47</v>
+      </c>
+      <c r="H18" t="s">
+        <v>53</v>
+      </c>
+      <c r="I18">
+        <v>32</v>
+      </c>
+      <c r="J18">
+        <v>32</v>
+      </c>
+      <c r="K18" t="s">
+        <v>71</v>
       </c>
       <c r="L18">
         <v>0</v>
@@ -1254,28 +1305,283 @@
       <c r="A19" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="B19" t="s">
+        <v>47</v>
+      </c>
       <c r="C19" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="E19">
+        <v>34</v>
+      </c>
+      <c r="F19" t="s">
+        <v>65</v>
+      </c>
+      <c r="G19" t="s">
+        <v>47</v>
+      </c>
+      <c r="H19" t="s">
+        <v>53</v>
+      </c>
+      <c r="I19">
+        <v>32</v>
+      </c>
+      <c r="J19">
+        <v>32</v>
+      </c>
+      <c r="K19" t="s">
+        <v>71</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20">
+        <v>45</v>
+      </c>
+      <c r="E20">
+        <v>45</v>
+      </c>
+      <c r="F20" t="s">
+        <v>66</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>1</v>
+      </c>
+      <c r="O20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21">
+        <v>46</v>
+      </c>
+      <c r="E21">
+        <v>50</v>
+      </c>
+      <c r="F21" t="s">
+        <v>67</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22">
+        <v>14</v>
+      </c>
+      <c r="E22">
         <v>35</v>
       </c>
-      <c r="F19" t="s">
-        <v>56</v>
-      </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
-      <c r="M19">
-        <v>1</v>
-      </c>
-      <c r="N19">
-        <v>0</v>
-      </c>
-      <c r="O19">
+      <c r="F22" t="s">
+        <v>60</v>
+      </c>
+      <c r="G22" t="s">
+        <v>49</v>
+      </c>
+      <c r="H22" t="s">
+        <v>54</v>
+      </c>
+      <c r="I22">
+        <v>14</v>
+      </c>
+      <c r="J22">
+        <v>35</v>
+      </c>
+      <c r="K22" t="s">
+        <v>60</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>1</v>
+      </c>
+      <c r="O22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23">
+        <v>14</v>
+      </c>
+      <c r="E23">
+        <v>35</v>
+      </c>
+      <c r="F23" t="s">
+        <v>60</v>
+      </c>
+      <c r="G23" t="s">
+        <v>50</v>
+      </c>
+      <c r="H23" t="s">
+        <v>54</v>
+      </c>
+      <c r="I23">
+        <v>14</v>
+      </c>
+      <c r="J23">
+        <v>35</v>
+      </c>
+      <c r="K23" t="s">
+        <v>60</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="O23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24">
+        <v>14</v>
+      </c>
+      <c r="E24">
+        <v>35</v>
+      </c>
+      <c r="F24" t="s">
+        <v>60</v>
+      </c>
+      <c r="G24" t="s">
+        <v>51</v>
+      </c>
+      <c r="H24" t="s">
+        <v>54</v>
+      </c>
+      <c r="I24">
+        <v>14</v>
+      </c>
+      <c r="J24">
+        <v>35</v>
+      </c>
+      <c r="K24" t="s">
+        <v>60</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>1</v>
+      </c>
+      <c r="O24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25">
+        <v>46</v>
+      </c>
+      <c r="E25">
+        <v>50</v>
+      </c>
+      <c r="F25" t="s">
+        <v>67</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>1</v>
+      </c>
+      <c r="O25">
         <v>1</v>
       </c>
     </row>

</xml_diff>